<commit_message>
Rest for the day
</commit_message>
<xml_diff>
--- a/Classifier1/Smote/Forest/Forrestweight_StatsPain.xlsx
+++ b/Classifier1/Smote/Forest/Forrestweight_StatsPain.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Documents\MedHelpCrawler_1\Classifier1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Documents\MedHelpCrawler_1\Classifier1\Smote\Forest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -129,6 +129,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pain Stats</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> With SMOTE</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -162,8 +192,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -180,7 +210,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -189,9 +219,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$20</c:f>
               <c:numCache>
@@ -256,8 +298,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$20</c:f>
               <c:numCache>
@@ -322,7 +364,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -340,7 +382,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -349,9 +391,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$20</c:f>
               <c:numCache>
@@ -416,8 +470,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$20</c:f>
               <c:numCache>
@@ -482,7 +536,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -500,7 +554,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -509,9 +563,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$20</c:f>
               <c:numCache>
@@ -576,8 +642,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$20</c:f>
               <c:numCache>
@@ -642,7 +708,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -660,7 +726,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -669,9 +735,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$20</c:f>
               <c:numCache>
@@ -736,8 +814,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$20</c:f>
               <c:numCache>
@@ -802,7 +880,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -813,17 +891,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="-1152568336"/>
-        <c:axId val="-1152578128"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-1152568336"/>
+        <c:axId val="1353712288"/>
+        <c:axId val="1353706304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1353712288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -833,8 +924,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -861,15 +952,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1152578128"/>
+        <c:crossAx val="1353706304"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="-1152578128"/>
+        <c:axId val="1353706304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,8 +983,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -920,9 +1014,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1152568336"/>
+        <c:crossAx val="1353712288"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1042,7 +1136,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1069,8 +1163,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1150,11 +1244,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1165,11 +1254,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1181,7 +1265,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1201,9 +1285,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1216,10 +1297,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1259,22 +1340,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1379,8 +1461,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1512,19 +1594,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1538,6 +1621,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1574,7 +1668,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1881,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>